<commit_message>
putting some functions in
</commit_message>
<xml_diff>
--- a/inst/extdata/pop_wo_com.xlsx
+++ b/inst/extdata/pop_wo_com.xlsx
@@ -1882,7 +1882,7 @@
     <t xml:space="preserve">Orkdal</t>
   </si>
   <si>
-    <t xml:space="preserve">municip1637</t>
+    <t xml:space="preserve">municip1638</t>
   </si>
   <si>
     <t xml:space="preserve">Roeros</t>
@@ -2008,7 +2008,7 @@
     <t xml:space="preserve">Lierne</t>
   </si>
   <si>
-    <t xml:space="preserve">municip1737</t>
+    <t xml:space="preserve">municip1738</t>
   </si>
   <si>
     <t xml:space="preserve">Roeyrvik</t>
@@ -2696,15 +2696,15 @@
   </sheetPr>
   <dimension ref="A1:C429"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A401" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C430" activeCellId="0" sqref="C430"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A317" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C331" activeCellId="0" sqref="C331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6337,7 +6337,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
         <v>661</v>
       </c>

</xml_diff>